<commit_message>
Started creating the battery module, will work on the payload tomorrow
</commit_message>
<xml_diff>
--- a/user/userinput.xlsx
+++ b/user/userinput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KILKISZenbook\Documents\Python\KBE\user\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F868F7-447E-4260-8A65-771BFDB0327C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9172EA1-E86B-44C2-870A-2CEADC6A7C28}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -794,7 +794,7 @@
   <dimension ref="B1:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -846,7 +846,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="21">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="D5" s="7" t="str">
         <f>IF(B5="Endurance","[h]","[km]")</f>
@@ -859,17 +859,17 @@
     </row>
     <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="22">
-        <v>0.25</v>
+        <v>20</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="12" t="str">
         <f>IF(B6=Options!E2,Options!J3,Options!J4)</f>
-        <v>Desired Range expressed in Kilometers</v>
+        <v>Desired Payload Weight (Mass) expressed in Kilograms</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="B2" s="24">
         <f>Inputs!C5</f>
-        <v>1.2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1174,7 +1174,7 @@
       </c>
       <c r="B3" s="24" t="str">
         <f>IF(Inputs!B6=Options!E2,Options!F2,Options!F3)</f>
-        <v>payload</v>
+        <v>mtow</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="B4" s="24">
         <f>Inputs!C6</f>
-        <v>0.25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Started implementing boom possibility into the code
</commit_message>
<xml_diff>
--- a/user/userinput.xlsx
+++ b/user/userinput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KILKISZenbook\Documents\Python\KBE\user\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9172EA1-E86B-44C2-870A-2CEADC6A7C28}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11468CC7-36A4-4DFA-BE19-635462593F92}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -794,7 +794,7 @@
   <dimension ref="B1:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1140,7 +1140,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added some minor bug-fixes and attempted to create a more realistic UAV instatiation with the default values. Creating a proper fuselage, and fixing the vertical tail is of priority to make this a reality
</commit_message>
<xml_diff>
--- a/user/userinput.xlsx
+++ b/user/userinput.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KILKISZenbook\Documents\Python\KBE\user\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11468CC7-36A4-4DFA-BE19-635462593F92}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B47423-C7EB-4A21-8242-F94CC146D133}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,9 +64,6 @@
     <t>Configuration</t>
   </si>
   <si>
-    <t>Vector containing outer dimensions of payload [length, width, height]</t>
-  </si>
-  <si>
     <t>Aircraft Configuration (Current supported types: Conventional, Canard, Flying Wing, Twin-Boom)</t>
   </si>
   <si>
@@ -200,6 +197,9 @@
   </si>
   <si>
     <t>target_value</t>
+  </si>
+  <si>
+    <t>Specifier for the Type of Payload (Gimbaled Camera, Synethic Aperature Radar)</t>
   </si>
 </sst>
 </file>
@@ -534,22 +534,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2166110</xdr:colOff>
+      <xdr:colOff>2095500</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>16565</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>17809</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>20782</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Side view of a sports car">
+        <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CA3B692-8A8A-4998-8605-5DB1924E57A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -571,8 +571,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6365393" y="16565"/>
-          <a:ext cx="3765481" cy="1727407"/>
+          <a:off x="5886450" y="9525"/>
+          <a:ext cx="3838575" cy="1744807"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -794,7 +794,7 @@
   <dimension ref="B1:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -859,13 +859,13 @@
     </row>
     <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="22">
         <v>20</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="12" t="str">
         <f>IF(B6=Options!E2,Options!J3,Options!J4)</f>
@@ -874,16 +874,16 @@
     </row>
     <row r="7" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -891,13 +891,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -908,24 +908,24 @@
         <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="19" t="b">
         <v>1</v>
       </c>
       <c r="D10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>11</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1003,98 +1003,98 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I2" s="15" t="b">
         <v>1</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I3" s="15" t="b">
         <v>0</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K3" s="16"/>
       <c r="L3" s="16"/>
@@ -1103,13 +1103,13 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K4" s="16"/>
       <c r="L4" s="16"/>
@@ -1118,13 +1118,13 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1152,7 +1152,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="24" t="str">
         <f>IF(Inputs!B5=Options!C2,Options!D2,Options!D3)</f>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="24">
         <f>Inputs!C5</f>
@@ -1170,7 +1170,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="24" t="str">
         <f>IF(Inputs!B6=Options!E2,Options!F2,Options!F3)</f>
@@ -1179,7 +1179,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="24">
         <f>Inputs!C6</f>
@@ -1188,7 +1188,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="24" t="str">
         <f>INDEX(Options!H2:H3, MATCH(Inputs!C7, Options!G2:G3))</f>
@@ -1197,7 +1197,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="24" t="str">
         <f>INDEX(Options!B:B, MATCH(Inputs!C8, Options!A:A,0))</f>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="24" t="str">
         <f>IF(Inputs!C9=Options!I2, "True", "False")</f>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="24" t="str">
         <f>IF(Inputs!C10=Options!I2, "True", "False")</f>

</xml_diff>

<commit_message>
Transformed input values from meter to km and second to hour
</commit_message>
<xml_diff>
--- a/user/userinput.xlsx
+++ b/user/userinput.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KILKISZenbook\Documents\Python\KBE\user\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B47423-C7EB-4A21-8242-F94CC146D133}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6DCB87-89C7-4E6D-97C9-CFF8B479B45B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
-    <sheet name="Options" sheetId="2" r:id="rId2"/>
-    <sheet name="export_ready_inputs" sheetId="3" r:id="rId3"/>
+    <sheet name="Options" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="export_ready_inputs" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ColumnTitle1">Inputs!$B$4</definedName>
-    <definedName name="InputArea">Inputs!$B$5:$E$10</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Inputs!$4:$4</definedName>
-    <definedName name="RowTitleRegion1..C2">Inputs!$B$2</definedName>
+    <definedName name="ColumnTitle1">Inputs!$B$5</definedName>
+    <definedName name="InputArea">Inputs!$B$6:$E$10</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Inputs!$5:$5</definedName>
+    <definedName name="RowTitleRegion1..C2">Inputs!$B$3</definedName>
     <definedName name="RowTitleRegion2..C4">Inputs!#REF!</definedName>
     <definedName name="RowTitleRegion3..E4">Inputs!#REF!</definedName>
     <definedName name="Vehicle_1_Name">IF(RIGHT(Inputs!#REF!,5)="Total", TRIM(LEFT(Inputs!#REF!,SEARCH("TOTAL",Inputs!#REF!)-1)),Inputs!#REF!)</definedName>
-    <definedName name="Vehicle_2_Name">IF(RIGHT(Inputs!$B$3,5)="Total", TRIM(LEFT(Inputs!$B$3,SEARCH("TOTAL",Inputs!$B$3)-1)),Inputs!$B$3)</definedName>
+    <definedName name="Vehicle_2_Name">IF(RIGHT(Inputs!$B$4,5)="Total", TRIM(LEFT(Inputs!$B$4,SEARCH("TOTAL",Inputs!$B$4)-1)),Inputs!$B$4)</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>UAV Design Input File</t>
   </si>
@@ -64,18 +64,9 @@
     <t>Configuration</t>
   </si>
   <si>
-    <t>Aircraft Configuration (Current supported types: Conventional, Canard, Flying Wing, Twin-Boom)</t>
-  </si>
-  <si>
-    <t>Portable</t>
-  </si>
-  <si>
     <t>[-]</t>
   </si>
   <si>
-    <t>If there is a requirement for potability (foldable wings, or detachable elements)</t>
-  </si>
-  <si>
     <t>[kg]</t>
   </si>
   <si>
@@ -85,15 +76,6 @@
     <t>Conventional</t>
   </si>
   <si>
-    <t>Canard</t>
-  </si>
-  <si>
-    <t>Flying-Wing</t>
-  </si>
-  <si>
-    <t>Twin-Boom</t>
-  </si>
-  <si>
     <t>Endurance/Range</t>
   </si>
   <si>
@@ -109,15 +91,6 @@
     <t>conventional</t>
   </si>
   <si>
-    <t>canard</t>
-  </si>
-  <si>
-    <t>flyingwing</t>
-  </si>
-  <si>
-    <t>twinboom</t>
-  </si>
-  <si>
     <t>Prompts</t>
   </si>
   <si>
@@ -163,9 +136,6 @@
     <t>handlaunch</t>
   </si>
   <si>
-    <t>portable</t>
-  </si>
-  <si>
     <t>Payload Type</t>
   </si>
   <si>
@@ -175,18 +145,12 @@
     <t>EO/IR Camera</t>
   </si>
   <si>
-    <t>Synthetic Aperature Radar</t>
-  </si>
-  <si>
     <t>payload_type</t>
   </si>
   <si>
     <t>eoir</t>
   </si>
   <si>
-    <t>sar</t>
-  </si>
-  <si>
     <t>performance_goal</t>
   </si>
   <si>
@@ -200,6 +164,9 @@
   </si>
   <si>
     <t>Specifier for the Type of Payload (Gimbaled Camera, Synethic Aperature Radar)</t>
+  </si>
+  <si>
+    <t>Aircraft Configuration (Current supported types: Conventional)</t>
   </si>
 </sst>
 </file>
@@ -302,7 +269,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -368,17 +335,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -408,7 +364,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -423,9 +379,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -444,9 +397,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -460,9 +410,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -478,6 +425,18 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -535,13 +494,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2095500</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>20782</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -791,10 +750,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:E11"/>
+  <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -807,129 +766,115 @@
     <col min="6" max="6" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="5" t="s">
+    <row r="2" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C5" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+    <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C6" s="18">
         <v>2</v>
       </c>
-      <c r="D5" s="7" t="str">
-        <f>IF(B5="Endurance","[h]","[km]")</f>
+      <c r="D6" s="6" t="str">
+        <f>IF(B6="Endurance","[h]","[km]")</f>
         <v>[h]</v>
       </c>
-      <c r="E5" s="7" t="str">
-        <f>IF(B5=Options!C2,Options!J2,Options!J3)</f>
+      <c r="E6" s="6" t="str">
+        <f>IF(B6=Options!C2,Options!J2,Options!J3)</f>
         <v>Desired Endurance expressed in Hours</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="22">
+    <row r="7" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="19">
         <v>20</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="12" t="str">
-        <f>IF(B6=Options!E2,Options!J3,Options!J4)</f>
+      <c r="D7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="11" t="str">
+        <f>IF(B7=Options!E2,Options!J3,Options!J4)</f>
         <v>Desired Payload Weight (Mass) expressed in Kilograms</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+    <row r="8" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="12" t="s">
+    </row>
+    <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="20" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>11</v>
+      <c r="E10" s="20" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
+      <c r="B11" s="8"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -946,31 +891,31 @@
           <x14:formula1>
             <xm:f>Options!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C7</xm:sqref>
+          <xm:sqref>C8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{71BC174E-0564-4645-9BC1-A86F452C0ED6}">
           <x14:formula1>
             <xm:f>Options!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B5</xm:sqref>
+          <xm:sqref>B6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5CBA5A40-00F0-4718-8708-C5E23D6A6C67}">
           <x14:formula1>
             <xm:f>Options!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C8</xm:sqref>
+          <xm:sqref>C9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2FA691A5-8663-41A4-BFBA-EC0FAA1107A9}">
           <x14:formula1>
             <xm:f>Options!$I$2:$I$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C9:C10</xm:sqref>
+          <xm:sqref>C10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{296B8092-F3D5-43BB-B0FF-E3E12613CCC8}">
           <x14:formula1>
             <xm:f>Options!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B6</xm:sqref>
+          <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -983,152 +928,128 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="18" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" style="18" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="15" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="1" width="20.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" style="16" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="14" t="s">
+      <c r="D3" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="14" t="s">
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="18" t="s">
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M11" s="16"/>
+      <c r="M11" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1137,87 +1058,78 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00611EDB-69E9-45D7-ACBF-9FAFDB386819}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="24" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="17.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="21" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="24" t="str">
-        <f>IF(Inputs!B5=Options!C2,Options!D2,Options!D3)</f>
+      <c r="A1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="21" t="str">
+        <f>IF(Inputs!B6=Options!C2,Options!D2,Options!D3)</f>
         <v>endurance</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="24">
-        <f>Inputs!C5</f>
+      <c r="A2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="21">
+        <f>Inputs!C6</f>
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="24" t="str">
-        <f>IF(Inputs!B6=Options!E2,Options!F2,Options!F3)</f>
+      <c r="A3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="21" t="str">
+        <f>IF(Inputs!B7=Options!E2,Options!F2,Options!F3)</f>
         <v>mtow</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="24">
-        <f>Inputs!C6</f>
+      <c r="A4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="21">
+        <f>Inputs!C7</f>
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="24" t="str">
-        <f>INDEX(Options!H2:H3, MATCH(Inputs!C7, Options!G2:G3))</f>
+      <c r="A5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="21" t="str">
+        <f>INDEX(Options!H2:H3, MATCH(Inputs!C8, Options!G2:G3))</f>
         <v>eoir</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="24" t="str">
-        <f>INDEX(Options!B:B, MATCH(Inputs!C8, Options!A:A,0))</f>
+      <c r="A6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="21" t="str">
+        <f>INDEX(Options!B:B, MATCH(Inputs!C9, Options!A:A,0))</f>
         <v>conventional</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="24" t="str">
-        <f>IF(Inputs!C9=Options!I2, "True", "False")</f>
-        <v>True</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="24" t="str">
+      <c r="A7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="21" t="str">
         <f>IF(Inputs!C10=Options!I2, "True", "False")</f>
         <v>True</v>
       </c>

</xml_diff>

<commit_message>
problem found with excel sheet 'configuration'
</commit_message>
<xml_diff>
--- a/user/userinput.xlsx
+++ b/user/userinput.xlsx
@@ -5,17 +5,17 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KILKISZenbook\Documents\Python\KBE\user\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nlsnj\Documents\TU Delft Master Flight Performance\Period 4\AE4204 Knowledge Based Engineering\Assignment\Python Files\KBE\user\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6DCB87-89C7-4E6D-97C9-CFF8B479B45B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D8265D-95FF-4B27-AA53-D2CABAEF77B6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
-    <sheet name="Options" sheetId="2" state="hidden" r:id="rId2"/>
-    <sheet name="export_ready_inputs" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="Options" sheetId="2" r:id="rId2"/>
+    <sheet name="export_ready_inputs" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="ColumnTitle1">Inputs!$B$5</definedName>
@@ -752,21 +752,21 @@
   </sheetPr>
   <dimension ref="B2:E11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="88.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="88.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -774,19 +774,19 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
@@ -800,7 +800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="22" t="s">
         <v>4</v>
       </c>
@@ -816,7 +816,7 @@
         <v>Desired Endurance expressed in Hours</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
         <v>22</v>
       </c>
@@ -831,7 +831,7 @@
         <v>Desired Payload Weight (Mass) expressed in Kilograms</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>32</v>
       </c>
@@ -845,7 +845,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="11" t="s">
         <v>7</v>
       </c>
@@ -859,7 +859,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="20" t="s">
         <v>6</v>
       </c>
@@ -873,7 +873,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="8"/>
     </row>
   </sheetData>
@@ -927,26 +927,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587AF12F-E22C-49AF-B91A-32B9F55651C7}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="16" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" style="16" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="13" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="20.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="25.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.33203125" style="16" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>10</v>
       </c>
@@ -978,7 +978,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>11</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C3" s="13" t="s">
         <v>13</v>
       </c>
@@ -1034,7 +1034,7 @@
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="J4" s="8" t="s">
         <v>29</v>
       </c>
@@ -1043,12 +1043,12 @@
       <c r="M4" s="14"/>
       <c r="N4" s="14"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="J5" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="M11" s="14"/>
     </row>
   </sheetData>
@@ -1061,17 +1061,17 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="21" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="17.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" style="21" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>endurance</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>39</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>mtow</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>35</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>eoir</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>30</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>conventional</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Added a way to disable user input form child classes, when they aren't run as the main file and polished up the parameter generator class
</commit_message>
<xml_diff>
--- a/user/userinput.xlsx
+++ b/user/userinput.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nlsnj\Documents\TU Delft Master Flight Performance\Period 4\AE4204 Knowledge Based Engineering\Assignment\Python Files\KBE\user\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KILKISZenbook\Documents\Python\KBE\user\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D8265D-95FF-4B27-AA53-D2CABAEF77B6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C55B78-D435-4BD4-93EA-760CE0804BE4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -752,21 +752,21 @@
   </sheetPr>
   <dimension ref="B2:E11"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="88.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="88.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -774,19 +774,19 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
@@ -800,7 +800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
         <v>4</v>
       </c>
@@ -816,22 +816,22 @@
         <v>Desired Endurance expressed in Hours</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="19">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="11" t="str">
         <f>IF(B7=Options!E2,Options!J3,Options!J4)</f>
-        <v>Desired Payload Weight (Mass) expressed in Kilograms</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>Desired Range expressed in Kilometers</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>32</v>
       </c>
@@ -845,7 +845,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>7</v>
       </c>
@@ -859,12 +859,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>8</v>
@@ -873,7 +873,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
     </row>
   </sheetData>
@@ -927,26 +927,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587AF12F-E22C-49AF-B91A-32B9F55651C7}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" style="16" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="25.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.33203125" style="16" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="13"/>
+    <col min="1" max="1" width="20.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" style="16" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>10</v>
       </c>
@@ -978,7 +978,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>11</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C3" s="13" t="s">
         <v>13</v>
       </c>
@@ -1034,7 +1034,7 @@
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J4" s="8" t="s">
         <v>29</v>
       </c>
@@ -1043,12 +1043,12 @@
       <c r="M4" s="14"/>
       <c r="N4" s="14"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J5" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M11" s="14"/>
     </row>
   </sheetData>
@@ -1064,14 +1064,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" style="21" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="7"/>
+    <col min="1" max="1" width="17.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="21" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>endurance</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>39</v>
       </c>
@@ -1089,25 +1089,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="21" t="str">
         <f>IF(Inputs!B7=Options!E2,Options!F2,Options!F3)</f>
-        <v>mtow</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>payload</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B4" s="21">
         <f>Inputs!C7</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>35</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>eoir</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>30</v>
       </c>
@@ -1125,13 +1125,13 @@
         <v>conventional</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="21" t="str">
         <f>IF(Inputs!C10=Options!I2, "True", "False")</f>
-        <v>True</v>
+        <v>False</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed excel sheet as well as excel export
</commit_message>
<xml_diff>
--- a/user/userinput.xlsx
+++ b/user/userinput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KILKISZenbook\Documents\Python\KBE\user\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C55B78-D435-4BD4-93EA-760CE0804BE4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CEE633-3CD3-45DE-A089-B8E1DFA1B96D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -753,7 +753,7 @@
   <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -827,8 +827,8 @@
         <v>9</v>
       </c>
       <c r="E7" s="11" t="str">
-        <f>IF(B7=Options!E2,Options!J3,Options!J4)</f>
-        <v>Desired Range expressed in Kilometers</v>
+        <f>IF(B7=Options!E2,Options!J4,Options!J5)</f>
+        <v>Desired Payload Weight (Mass) expressed in Kilograms</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -928,7 +928,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>